<commit_message>
- added UML diagrams - added Use Case diagrams - added Activity Diagrams - updated SRS
</commit_message>
<xml_diff>
--- a/gantt-chart/SWYL-Gantt-Chart.xlsx
+++ b/gantt-chart/SWYL-Gantt-Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/logann131/coding/web-dev/SWYL/documentation/gantt-chart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE6D3C7-03EA-C848-9BC1-14EF5D3FF9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBAF59B-2E65-9243-8ABA-2B3191AF98F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -1687,12 +1687,6 @@
     <xf numFmtId="164" fontId="28" fillId="27" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1707,6 +1701,12 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2266,9 +2266,9 @@
   </sheetPr>
   <dimension ref="A1:DH122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="120" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK18" sqref="AK18"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF24" sqref="AF24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2292,27 +2292,27 @@
       <c r="E1" s="44"/>
       <c r="G1" s="1"/>
       <c r="H1" s="7"/>
-      <c r="I1" s="154" t="str">
+      <c r="I1" s="159" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToMakeAGanttChart","")</f>
         <v/>
       </c>
-      <c r="J1" s="155"/>
-      <c r="K1" s="155"/>
-      <c r="L1" s="155"/>
-      <c r="M1" s="155"/>
-      <c r="N1" s="155"/>
-      <c r="O1" s="155"/>
-      <c r="P1" s="155"/>
-      <c r="Q1" s="155"/>
-      <c r="R1" s="155"/>
-      <c r="S1" s="155"/>
-      <c r="T1" s="155"/>
-      <c r="U1" s="155"/>
-      <c r="V1" s="155"/>
-      <c r="W1" s="155"/>
-      <c r="X1" s="155"/>
-      <c r="Y1" s="155"/>
-      <c r="Z1" s="155"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
+      <c r="M1" s="160"/>
+      <c r="N1" s="160"/>
+      <c r="O1" s="160"/>
+      <c r="P1" s="160"/>
+      <c r="Q1" s="160"/>
+      <c r="R1" s="160"/>
+      <c r="S1" s="160"/>
+      <c r="T1" s="160"/>
+      <c r="U1" s="160"/>
+      <c r="V1" s="160"/>
+      <c r="W1" s="160"/>
+      <c r="X1" s="160"/>
+      <c r="Y1" s="160"/>
+      <c r="Z1" s="160"/>
     </row>
     <row r="2" spans="1:112" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
@@ -2321,21 +2321,21 @@
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="159">
+      <c r="D2" s="157">
         <v>44795</v>
       </c>
-      <c r="E2" s="160"/>
+      <c r="E2" s="158"/>
     </row>
     <row r="3" spans="1:112" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
       <c r="C3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="159">
+      <c r="D3" s="157">
         <f ca="1">TODAY()</f>
         <v>44827</v>
       </c>
-      <c r="E3" s="160"/>
+      <c r="E3" s="158"/>
     </row>
     <row r="4" spans="1:112" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
@@ -2344,156 +2344,156 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="H4" s="156">
+      <c r="H4" s="154">
         <f>H5</f>
         <v>44795</v>
       </c>
-      <c r="I4" s="157"/>
-      <c r="J4" s="157"/>
-      <c r="K4" s="157"/>
-      <c r="L4" s="157"/>
-      <c r="M4" s="157"/>
-      <c r="N4" s="158"/>
-      <c r="O4" s="156">
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
+      <c r="K4" s="155"/>
+      <c r="L4" s="155"/>
+      <c r="M4" s="155"/>
+      <c r="N4" s="156"/>
+      <c r="O4" s="154">
         <f>O5</f>
         <v>44802</v>
       </c>
-      <c r="P4" s="157"/>
-      <c r="Q4" s="157"/>
-      <c r="R4" s="157"/>
-      <c r="S4" s="157"/>
-      <c r="T4" s="157"/>
-      <c r="U4" s="158"/>
-      <c r="V4" s="156">
+      <c r="P4" s="155"/>
+      <c r="Q4" s="155"/>
+      <c r="R4" s="155"/>
+      <c r="S4" s="155"/>
+      <c r="T4" s="155"/>
+      <c r="U4" s="156"/>
+      <c r="V4" s="154">
         <f>V5</f>
         <v>44809</v>
       </c>
-      <c r="W4" s="157"/>
-      <c r="X4" s="157"/>
-      <c r="Y4" s="157"/>
-      <c r="Z4" s="157"/>
-      <c r="AA4" s="157"/>
-      <c r="AB4" s="158"/>
-      <c r="AC4" s="156">
+      <c r="W4" s="155"/>
+      <c r="X4" s="155"/>
+      <c r="Y4" s="155"/>
+      <c r="Z4" s="155"/>
+      <c r="AA4" s="155"/>
+      <c r="AB4" s="156"/>
+      <c r="AC4" s="154">
         <f>AC5</f>
         <v>44816</v>
       </c>
-      <c r="AD4" s="157"/>
-      <c r="AE4" s="157"/>
-      <c r="AF4" s="157"/>
-      <c r="AG4" s="157"/>
-      <c r="AH4" s="157"/>
-      <c r="AI4" s="158"/>
-      <c r="AJ4" s="156">
+      <c r="AD4" s="155"/>
+      <c r="AE4" s="155"/>
+      <c r="AF4" s="155"/>
+      <c r="AG4" s="155"/>
+      <c r="AH4" s="155"/>
+      <c r="AI4" s="156"/>
+      <c r="AJ4" s="154">
         <f>AJ5</f>
         <v>44823</v>
       </c>
-      <c r="AK4" s="157"/>
-      <c r="AL4" s="157"/>
-      <c r="AM4" s="157"/>
-      <c r="AN4" s="157"/>
-      <c r="AO4" s="157"/>
-      <c r="AP4" s="158"/>
-      <c r="AQ4" s="156">
+      <c r="AK4" s="155"/>
+      <c r="AL4" s="155"/>
+      <c r="AM4" s="155"/>
+      <c r="AN4" s="155"/>
+      <c r="AO4" s="155"/>
+      <c r="AP4" s="156"/>
+      <c r="AQ4" s="154">
         <f>AQ5</f>
         <v>44830</v>
       </c>
-      <c r="AR4" s="157"/>
-      <c r="AS4" s="157"/>
-      <c r="AT4" s="157"/>
-      <c r="AU4" s="157"/>
-      <c r="AV4" s="157"/>
-      <c r="AW4" s="158"/>
-      <c r="AX4" s="156">
+      <c r="AR4" s="155"/>
+      <c r="AS4" s="155"/>
+      <c r="AT4" s="155"/>
+      <c r="AU4" s="155"/>
+      <c r="AV4" s="155"/>
+      <c r="AW4" s="156"/>
+      <c r="AX4" s="154">
         <f>AX5</f>
         <v>44837</v>
       </c>
-      <c r="AY4" s="157"/>
-      <c r="AZ4" s="157"/>
-      <c r="BA4" s="157"/>
-      <c r="BB4" s="157"/>
-      <c r="BC4" s="157"/>
-      <c r="BD4" s="158"/>
-      <c r="BE4" s="156">
+      <c r="AY4" s="155"/>
+      <c r="AZ4" s="155"/>
+      <c r="BA4" s="155"/>
+      <c r="BB4" s="155"/>
+      <c r="BC4" s="155"/>
+      <c r="BD4" s="156"/>
+      <c r="BE4" s="154">
         <f>BE5</f>
         <v>44844</v>
       </c>
-      <c r="BF4" s="157"/>
-      <c r="BG4" s="157"/>
-      <c r="BH4" s="157"/>
-      <c r="BI4" s="157"/>
-      <c r="BJ4" s="157"/>
-      <c r="BK4" s="158"/>
-      <c r="BL4" s="156">
+      <c r="BF4" s="155"/>
+      <c r="BG4" s="155"/>
+      <c r="BH4" s="155"/>
+      <c r="BI4" s="155"/>
+      <c r="BJ4" s="155"/>
+      <c r="BK4" s="156"/>
+      <c r="BL4" s="154">
         <f>BL5</f>
         <v>44851</v>
       </c>
-      <c r="BM4" s="157"/>
-      <c r="BN4" s="157"/>
-      <c r="BO4" s="157"/>
-      <c r="BP4" s="157"/>
-      <c r="BQ4" s="157"/>
-      <c r="BR4" s="158"/>
-      <c r="BS4" s="156">
+      <c r="BM4" s="155"/>
+      <c r="BN4" s="155"/>
+      <c r="BO4" s="155"/>
+      <c r="BP4" s="155"/>
+      <c r="BQ4" s="155"/>
+      <c r="BR4" s="156"/>
+      <c r="BS4" s="154">
         <f>BS5</f>
         <v>44858</v>
       </c>
-      <c r="BT4" s="157"/>
-      <c r="BU4" s="157"/>
-      <c r="BV4" s="157"/>
-      <c r="BW4" s="157"/>
-      <c r="BX4" s="157"/>
-      <c r="BY4" s="158"/>
-      <c r="BZ4" s="156">
+      <c r="BT4" s="155"/>
+      <c r="BU4" s="155"/>
+      <c r="BV4" s="155"/>
+      <c r="BW4" s="155"/>
+      <c r="BX4" s="155"/>
+      <c r="BY4" s="156"/>
+      <c r="BZ4" s="154">
         <f>BZ5</f>
         <v>44865</v>
       </c>
-      <c r="CA4" s="157"/>
-      <c r="CB4" s="157"/>
-      <c r="CC4" s="157"/>
-      <c r="CD4" s="157"/>
-      <c r="CE4" s="157"/>
-      <c r="CF4" s="158"/>
-      <c r="CG4" s="156">
+      <c r="CA4" s="155"/>
+      <c r="CB4" s="155"/>
+      <c r="CC4" s="155"/>
+      <c r="CD4" s="155"/>
+      <c r="CE4" s="155"/>
+      <c r="CF4" s="156"/>
+      <c r="CG4" s="154">
         <f>CG5</f>
         <v>44872</v>
       </c>
-      <c r="CH4" s="157"/>
-      <c r="CI4" s="157"/>
-      <c r="CJ4" s="157"/>
-      <c r="CK4" s="157"/>
-      <c r="CL4" s="157"/>
-      <c r="CM4" s="158"/>
-      <c r="CN4" s="156">
+      <c r="CH4" s="155"/>
+      <c r="CI4" s="155"/>
+      <c r="CJ4" s="155"/>
+      <c r="CK4" s="155"/>
+      <c r="CL4" s="155"/>
+      <c r="CM4" s="156"/>
+      <c r="CN4" s="154">
         <f>CN5</f>
         <v>44879</v>
       </c>
-      <c r="CO4" s="157"/>
-      <c r="CP4" s="157"/>
-      <c r="CQ4" s="157"/>
-      <c r="CR4" s="157"/>
-      <c r="CS4" s="157"/>
-      <c r="CT4" s="158"/>
-      <c r="CU4" s="156">
+      <c r="CO4" s="155"/>
+      <c r="CP4" s="155"/>
+      <c r="CQ4" s="155"/>
+      <c r="CR4" s="155"/>
+      <c r="CS4" s="155"/>
+      <c r="CT4" s="156"/>
+      <c r="CU4" s="154">
         <f>CU5</f>
         <v>44886</v>
       </c>
-      <c r="CV4" s="157"/>
-      <c r="CW4" s="157"/>
-      <c r="CX4" s="157"/>
-      <c r="CY4" s="157"/>
-      <c r="CZ4" s="157"/>
-      <c r="DA4" s="158"/>
-      <c r="DB4" s="156">
+      <c r="CV4" s="155"/>
+      <c r="CW4" s="155"/>
+      <c r="CX4" s="155"/>
+      <c r="CY4" s="155"/>
+      <c r="CZ4" s="155"/>
+      <c r="DA4" s="156"/>
+      <c r="DB4" s="154">
         <f>DB5</f>
         <v>44893</v>
       </c>
-      <c r="DC4" s="157"/>
-      <c r="DD4" s="157"/>
-      <c r="DE4" s="157"/>
-      <c r="DF4" s="157"/>
-      <c r="DG4" s="157"/>
-      <c r="DH4" s="158"/>
+      <c r="DC4" s="155"/>
+      <c r="DD4" s="155"/>
+      <c r="DE4" s="155"/>
+      <c r="DF4" s="155"/>
+      <c r="DG4" s="155"/>
+      <c r="DH4" s="156"/>
     </row>
     <row r="5" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
@@ -5076,7 +5076,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="51">
         <v>44827</v>
@@ -17071,6 +17071,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="I1:Z1"/>
+    <mergeCell ref="AJ4:AP4"/>
+    <mergeCell ref="AQ4:AW4"/>
+    <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BE4:BK4"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H4:N4"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="V4:AB4"/>
+    <mergeCell ref="AC4:AI4"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="CU4:DA4"/>
     <mergeCell ref="DB4:DH4"/>
     <mergeCell ref="BL4:BR4"/>
@@ -17078,17 +17089,6 @@
     <mergeCell ref="BZ4:CF4"/>
     <mergeCell ref="CG4:CM4"/>
     <mergeCell ref="CN4:CT4"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H4:N4"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="V4:AB4"/>
-    <mergeCell ref="AC4:AI4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="I1:Z1"/>
-    <mergeCell ref="AJ4:AP4"/>
-    <mergeCell ref="AQ4:AW4"/>
-    <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="BE4:BK4"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C118">
     <cfRule type="dataBar" priority="33">

</xml_diff>